<commit_message>
update stand nach labor
</commit_message>
<xml_diff>
--- a/Labor 1 Ergebnisse und Graphen.xlsx
+++ b/Labor 1 Ergebnisse und Graphen.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinarkarchevskii/Desktop/dhbw_dev/semester3/Messdatenerfassung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippgehrig/Desktop/dhbw/Studienjahr 2/Semester 3/Messdatenerfassung/Labor/Labor 1/LaTeX Berricht/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCD0812-EE3D-0F48-A581-9B827BCA9163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72853E8D-392A-4F4E-9287-5D8D8C4044A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4A0D7C32-F860-B045-B11A-99C13AEB249A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{4A0D7C32-F860-B045-B11A-99C13AEB249A}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrale Nichtlinearität" sheetId="1" r:id="rId1"/>
     <sheet name="Differenzielle Nichtlinearität" sheetId="2" r:id="rId2"/>
     <sheet name="Konversionszeit" sheetId="3" r:id="rId3"/>
+    <sheet name="Monotonie und Nichtlinearität" sheetId="4" r:id="rId4"/>
+    <sheet name="Einschwingverhalten" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Integrale Nichtlinearität'!$D$2:$D$17</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Erwarteter Spannungswert</t>
   </si>
@@ -53,9 +55,6 @@
     <t>tatsächlicher Spannungswert</t>
   </si>
   <si>
-    <t>Tatsächlicher Spannungswert</t>
-  </si>
-  <si>
     <t>DNL</t>
   </si>
   <si>
@@ -132,23 +131,60 @@
   </si>
   <si>
     <t>"11111111"</t>
+  </si>
+  <si>
+    <t>∆V in [mV]</t>
+  </si>
+  <si>
+    <t>Erwarteter Spannungswert in [V]</t>
+  </si>
+  <si>
+    <t>Tatsächlicher Spannungswert in [V]</t>
+  </si>
+  <si>
+    <t>Notizen</t>
+  </si>
+  <si>
+    <t>bit 5 vermutlich kaputt: 00010000 -&gt; Output = 0V</t>
+  </si>
+  <si>
+    <t>BITMUSTER  xi+1</t>
+  </si>
+  <si>
+    <t>BITMUSTER xi</t>
+  </si>
+  <si>
+    <t>MONTONIE</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>nein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000\V"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="00000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,27 +207,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -202,11 +239,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000\V"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000\V"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -883,8 +918,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10684933" y="928631"/>
-              <a:ext cx="4573441" cy="2739237"/>
+              <a:off x="10917496" y="1090579"/>
+              <a:ext cx="4554526" cy="2687716"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -918,14 +953,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E00BD67-58FF-C24F-828F-C39D3354CF0D}" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E00BD67-58FF-C24F-828F-C39D3354CF0D}" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E17" xr:uid="{1E00BD67-58FF-C24F-828F-C39D3354CF0D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{67A94B3E-BF9C-DE41-B186-6E78847DC8F5}" name="Digitaler Output" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{FAF9267E-DD82-604A-BBB4-50B2A475EFC4}" name="Erwarteter Spannungswert" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{67A94B3E-BF9C-DE41-B186-6E78847DC8F5}" name="Digitaler Output" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{FAF9267E-DD82-604A-BBB4-50B2A475EFC4}" name="Erwarteter Spannungswert in [V]" dataDxfId="1">
       <calculatedColumnFormula>B1+0.32</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CBC833C5-F835-E740-AF60-BEF05AF78997}" name="Tatsächlicher Spannungswert" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{CBC833C5-F835-E740-AF60-BEF05AF78997}" name="Tatsächlicher Spannungswert in [V]" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{962940AD-7301-4740-ADD3-72ECC3377F93}" name="Abweichung" dataDxfId="3">
       <calculatedColumnFormula>C2-B2</calculatedColumnFormula>
     </tableColumn>
@@ -1234,15 +1269,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A5E22A-057D-0E49-ADED-789EC45B45EC}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1251,16 +1286,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1274,12 +1309,12 @@
       <c r="C2" s="3">
         <v>0.32100000000000001</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <f>C2-B2</f>
         <v>1.0000000000000009E-3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1294,17 +1329,17 @@
       <c r="C3" s="3">
         <v>0.63900000000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D17" si="0">C3-B3</f>
         <v>-1.0000000000000009E-3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A17" si="1">A3+16</f>
+        <f t="shared" ref="A4:A16" si="1">A3+16</f>
         <v>48</v>
       </c>
       <c r="B4" s="3">
@@ -1314,12 +1349,12 @@
       <c r="C4" s="3">
         <v>0.96699999999999997</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>7.0000000000000062E-3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1334,12 +1369,12 @@
       <c r="C5" s="3">
         <v>1.2769999999999999</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>-3.0000000000001137E-3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1354,12 +1389,12 @@
       <c r="C6" s="3">
         <v>1.601</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>9.9999999999988987E-4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1374,12 +1409,12 @@
       <c r="C7" s="3">
         <v>1.9219999999999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>1.9999999999997797E-3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,12 +1429,12 @@
       <c r="C8" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,12 +1449,12 @@
       <c r="C9" s="3">
         <v>2.5659999999999998</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>5.9999999999997833E-3</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1434,12 +1469,12 @@
       <c r="C10" s="3">
         <v>2.887</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>7.0000000000001172E-3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1454,12 +1489,12 @@
       <c r="C11" s="3">
         <v>3.2029999999999998</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>3.0000000000001137E-3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1474,12 +1509,12 @@
       <c r="C12" s="3">
         <v>3.5339999999999998</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>1.4000000000000234E-2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1494,12 +1529,12 @@
       <c r="C13" s="3">
         <v>3.843</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>3.0000000000005578E-3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1514,12 +1549,12 @@
       <c r="C14" s="3">
         <v>4.1580000000000004</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>-1.9999999999988916E-3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1534,12 +1569,12 @@
       <c r="C15" s="3">
         <v>4.4829999999999997</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>3.0000000000001137E-3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1554,12 +1589,12 @@
       <c r="C16" s="3">
         <v>4.8019999999999996</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>1.9999999999997797E-3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1574,12 +1609,12 @@
       <c r="C17" s="3">
         <v>5.1189999999999998</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>-1.000000000000334E-3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1618,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1785,7 +1820,7 @@
         <v>2.6619999999999999</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1809,30 +1844,229 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2C31BA-F075-FC4F-B7D4-1B074C620C31}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>C2/10 -1</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9.75</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" si="0">C3/10 -1</f>
+        <v>-2.5000000000000022E-2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>9.75</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-2.5000000000000022E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="4">
+        <v>111</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>10000</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1111</v>
+      </c>
+      <c r="C6">
+        <v>-150</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>100000</v>
+      </c>
+      <c r="B7" s="4">
+        <v>11111</v>
+      </c>
+      <c r="C7">
+        <v>170</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B8" s="4">
+        <v>111111</v>
+      </c>
+      <c r="C8">
+        <v>170</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>10000000</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1111111</v>
+      </c>
+      <c r="C9">
+        <v>170</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EAD24C-FC57-3C45-B03B-95DF1772DF12}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>